<commit_message>
Added exception handling, annotations, and resolved the click sign logic.
</commit_message>
<xml_diff>
--- a/DailyHoroscopeDescription.xlsx
+++ b/DailyHoroscopeDescription.xlsx
@@ -1,97 +1,186 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syste\Documents\UiPath\AllHoroscopeSequence\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370207AC-D432-4827-9435-B7E9ABADFFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{400E901E-2F06-48F6-9556-D3BCADAEEA97}"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <x:bookViews>
+    <x:workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="0" activeTab="0" xr2:uid="{400E901E-2F06-48F6-9556-D3BCADAEEA97}"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+  </x:sheets>
+  <x:definedNames/>
+  <x:calcPr calcId="191029"/>
+  <x:extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+    </x:ext>
+    <x:ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
-</workbook>
+    </x:ext>
+  </x:extLst>
+</x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Zodiac description</t>
-  </si>
-  <si>
-    <t>Zodiac sign</t>
-  </si>
-</sst>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+  <x:si>
+    <x:t>ZodiacSign</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ZodiacDescription</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Aries</x:t>
+  </x:si>
+  <x:si>
+    <x:t>The focus will be mainly on your career goals today, you want to accomplish the maximum in least amount of time. Be patient and go by the saying that ‘good things come to those who wait’. You need to be a team player and work with the strengths and weaknesses of your fellow colleagues. Family front will be harmonious and content. You will be inclined towards spiritual matters today and will find peace in following religious practices.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Taurus</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">You will be preoccupied with meeting new people and socializing with family members and relatives. It is best to adapt with people and their habits as you cannot change everybody as per your patterns and routines. You will enjoy good health today. Continue with your diet and fitness regime to enjoy your increased stamina levels. Your professional pursuits are extremely rewarding today and you will feel content with your competencies at work. </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Gemini</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">You need to put in extra efforts to achieve success at work. Be consistent and sincere at your job and you will reap the results soon. Single prospects need to look within and introspect as to what they are looking for in a partner. Planetary alignments are such that you will face harmony at home. There will be peace at home and between family members today. Your health will be average today, try to eat freshly cooked nutritious meals. </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cancer</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">If you are going through an unpleasant situation then it is advisable to let time take its turn, things will get better in its due course. You need to be emotionally strong while putting your thoughts in front of your partner. Cancer children will be joyful and will spread positive vibes in their homes and surroundings. Pay attention to your family’s health along with yours. You will enjoy financial stability today as you will good returns on your previous investments. </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Leo</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">You will be inclined towards visiting charitable organizations and helping the less fortunate. Today you will be interested in changing the décor and appearance of your home. It may be asked from you to train your subordinates on various workplace policies and procedures. Plan a day out with your spouse and participate in fun activities. Leo sun sign natives will flourish in their studies and perform well in their assessments. </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Virgo</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">It is important to maintain your emotional health along with your physical well-being. Practice yoga and deep breathing techniques to conserve your inner peace. Try to incorporate others into your busy schedule, spend some time with your parents and friends and share your feelings. You are focused on an overall growth at work today and will try to learn different techniques in order to perform better. Students pursuing higher education will remain dedicated to their studies. </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Libra</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">The day will be focused on solving various family issues and you need to be patient and have a gentle outlook towards resolving the situation. You will be energetic and aggressive in approaching your work responsibilities. The relationship with your spouse will be very supportive and understanding. Financially, you will be able to cater your family’s monetary needs and wants. As per the Libra prediction, students pursuing higher education will win awards in seminars. </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Scorpio</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Your optimistic attitude will be appreciated by your seniors today. You will be concentrated on moving forward in your career. Don’t isolate yourself; take help from people whenever you feel stuck. Scorpio children will be well-behaved and will impress the elders with their behavior and mannerisms. You will embrace good health only if you are consistent with your workouts and take fresh nutritious foods. If you are planning to invest then it is ideal to wait for a day and take second opinion from experts. </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sagittarius</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Your colleagues will take your side today and will root for your hard work and sincerity. Try not to make huge investments today as it might lead you to cash crunch. You might feel exhausted today so it is advisable to take rest and recover. You will feel appreciated and loved by your partner, despite of some conflict, you both will find a way to pacify each other. If you are looking to sell your property then you need to negotiate well to get a good value. </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Capricorn</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Don’t get disheartened by obstacles and hurdles coming your way, they are the stepping stones to your success. You will find peace and content in your relationship with your spouse. Refrain yourself from making impulse purchases today and try to maintain a balance between your savings and spending. Take care of your health and take proper measures to strengthen your immunity. You will be high on following good moral and ethical values. </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Aquarius</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Students or the young ones are expected to have difference of opinion with their parents and teachers. Try not to offend anybody on a personal front as you will repent your actions later. Monetary losses are expected in certain business deals so tread carefully. Indulge yourself in reading spiritual or self mentoring books to gain wisdom from them. . You will be able to take time out to pursue your hobbies and interests.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Pisces</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">The effort you put in while giving your message across will save you from a lot of frustrations in the end particularly at work front. Using tact and perseverance will take you a long way today. Health related concerns will have some relief. Keep a little time for yourself and try to relax. Indulge in these religious activities and you may find that pursuing these interests bring you joy and harmony. Peace and calmness will prevail at home; family members will enjoy each other’s company. </x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="0" formatCode=""/>
+  </x:numFmts>
+  <x:fonts count="2" x14ac:knownFonts="1">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellStyleXfs>
+  <x:cellXfs count="3">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
-</styleSheet>
+    </x:ext>
+  </x:extLst>
+</x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -390,29 +479,132 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBC4BD13-0EAE-4980-A30B-34F51BAB2ACD}">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="39.36328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="128.36328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.54296875" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{BBC4BD13-0EAE-4980-A30B-34F51BAB2ACD}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:C1"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="B4" sqref="B4 B4:B4"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <x:cols>
+    <x:col min="1" max="1" width="39.363281" style="2" customWidth="1"/>
+    <x:col min="2" max="2" width="128.363281" style="2" customWidth="1"/>
+    <x:col min="3" max="3" width="39.542969" style="2" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <x:c r="A1" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:3">
+      <x:c r="A2" s="2" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B2" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:3">
+      <x:c r="A3" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B3" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:3">
+      <x:c r="A4" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B4" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:3">
+      <x:c r="A5" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B5" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:3">
+      <x:c r="A6" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B6" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:3">
+      <x:c r="A7" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B7" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:3">
+      <x:c r="A8" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B8" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:3">
+      <x:c r="A9" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B9" s="2" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:3">
+      <x:c r="A10" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B10" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:3">
+      <x:c r="A11" s="2" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B11" s="2" t="s">
+        <x:v>21</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:3">
+      <x:c r="A12" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B12" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:3">
+      <x:c r="A13" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B13" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>